<commit_message>
just finished total rushing yards
</commit_message>
<xml_diff>
--- a/jsonData.xlsx
+++ b/jsonData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15180" windowHeight="9168" tabRatio="974"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15180" windowHeight="9168" tabRatio="974" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="winloss" sheetId="2" r:id="rId1"/>
@@ -495,7 +495,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+    <sheetView zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
@@ -1468,7 +1468,7 @@
   <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1753,8 +1753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2524,7 +2524,7 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>